<commit_message>
Comparações entre numerico, experimental e analitco
</commit_message>
<xml_diff>
--- a/Projeto 1/Parte Experimental.xlsx
+++ b/Projeto 1/Parte Experimental.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Farinha\Documents\GitHub\MCL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alves\Desktop\MCL\Projeto 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406150E2-00E6-47A7-835A-220B8452F036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E74377-116E-455B-BC41-A7430DB8489F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="13452" yWindow="1020" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -760,7 +760,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -865,7 +865,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1022,7 +1022,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1208,7 +1208,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1246,7 +1246,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1186263888"/>
@@ -1325,7 +1325,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1363,7 +1363,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1756220544"/>
@@ -1411,7 +1411,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1492,7 +1492,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1597,7 +1597,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1748,7 +1748,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1923,7 +1923,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1961,7 +1961,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1186263888"/>
@@ -2045,7 +2045,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2083,7 +2083,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1756220544"/>
@@ -2131,7 +2131,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3636,32 +3636,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AH46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="2" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="7" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="35" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="24" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F2" s="23" t="s">
         <v>3</v>
       </c>
@@ -3676,7 +3676,7 @@
       <c r="O2" s="26"/>
       <c r="P2" s="26"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="6">
         <v>1</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>21468.698779218721</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <v>2</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>20395.263840257787</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="6">
         <v>3</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>20183.814356522787</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
         <v>4</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>20312.509173255636</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>20305.019309991156</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>19990.690345176823</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>20532.144805628643</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F11" s="10">
         <v>8</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>20388.467684362997</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="20" t="s">
         <v>15</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>19876.905328743498</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F13" s="10">
         <v>10</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>20084.433324521153</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F14" s="10">
         <v>11</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>19408.657104131118</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F15" s="10">
         <v>12</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>19959.120104637925</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F16" s="10">
         <v>13</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>18809.861249249603</v>
       </c>
     </row>
-    <row r="17" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F17" s="10">
         <v>14</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>19424.060800245512</v>
       </c>
     </row>
-    <row r="18" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F18" s="10">
         <v>15</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>15470.490902850406</v>
       </c>
     </row>
-    <row r="19" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F19" s="10">
         <v>16</v>
       </c>
@@ -4464,7 +4464,7 @@
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>
-    <row r="20" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:28" x14ac:dyDescent="0.3">
       <c r="F20" s="12">
         <v>17</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:28" x14ac:dyDescent="0.3">
       <c r="R21" s="21">
         <v>2</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>21.99905146258499</v>
       </c>
     </row>
-    <row r="22" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:28" x14ac:dyDescent="0.3">
       <c r="R22" s="1">
         <v>4</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>1.6198984403829184</v>
       </c>
     </row>
-    <row r="23" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:28" x14ac:dyDescent="0.3">
       <c r="R23" s="21">
         <v>7</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>4.6119783290310457</v>
       </c>
     </row>
-    <row r="24" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:28" x14ac:dyDescent="0.3">
       <c r="R24" s="1">
         <v>9</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>1.3613236351911095</v>
       </c>
     </row>
-    <row r="25" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:28" x14ac:dyDescent="0.3">
       <c r="R25" s="21">
         <v>12</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>2.6541976611501745</v>
       </c>
     </row>
-    <row r="26" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:28" x14ac:dyDescent="0.3">
       <c r="R26" s="1">
         <v>14</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>0.84417402480747006</v>
       </c>
     </row>
-    <row r="27" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:28" x14ac:dyDescent="0.3">
       <c r="R27" s="21">
         <v>17</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>1.6655292883579369</v>
       </c>
     </row>
-    <row r="28" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:28" x14ac:dyDescent="0.3">
       <c r="R28" s="1">
         <v>20</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>0.22359449234713161</v>
       </c>
     </row>
-    <row r="31" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:28" x14ac:dyDescent="0.3">
       <c r="U31" t="s">
         <v>27</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:28" x14ac:dyDescent="0.3">
       <c r="U32">
         <f>ABS(S21-N4)/S21*100</f>
         <v>12.046846655116159</v>
@@ -4695,7 +4695,7 @@
         <v>55.48957141087174</v>
       </c>
     </row>
-    <row r="33" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:34" x14ac:dyDescent="0.3">
       <c r="U33">
         <f t="shared" ref="U33:U38" si="3">ABS(S22-N5)/S22*100</f>
         <v>17.944049110648592</v>
@@ -4705,7 +4705,7 @@
         <v>23.841251566181029</v>
       </c>
     </row>
-    <row r="34" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:34" x14ac:dyDescent="0.3">
       <c r="U34">
         <f>ABS(S23-N6)/S23*100</f>
         <v>19.179653434664914</v>
@@ -4715,7 +4715,7 @@
         <v>27.885047535688994</v>
       </c>
     </row>
-    <row r="35" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:34" x14ac:dyDescent="0.3">
       <c r="U35">
         <f>ABS(S24-N7)/S24*100</f>
         <v>18.424561903321614</v>
@@ -4725,7 +4725,7 @@
         <v>20.521344998622034</v>
       </c>
     </row>
-    <row r="36" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:34" x14ac:dyDescent="0.3">
       <c r="U36">
         <f t="shared" si="3"/>
         <v>18.468244884473716</v>
@@ -4735,7 +4735,7 @@
         <v>23.939538273773241</v>
       </c>
     </row>
-    <row r="37" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:34" x14ac:dyDescent="0.3">
       <c r="U37">
         <f>ABS(S26-N9)/S26*100</f>
         <v>20.331012009316495</v>
@@ -4745,7 +4745,7 @@
         <v>19.769373680218155</v>
       </c>
     </row>
-    <row r="38" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:34" x14ac:dyDescent="0.3">
       <c r="N38" t="s">
         <v>17</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>21.019844901181209</v>
       </c>
     </row>
-    <row r="39" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:34" x14ac:dyDescent="0.3">
       <c r="H39">
         <v>35137</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>17.983363793685491</v>
       </c>
     </row>
-    <row r="41" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:34" x14ac:dyDescent="0.3">
       <c r="N41" t="s">
         <v>21</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:34" x14ac:dyDescent="0.3">
       <c r="N42">
         <f>AVERAGE(R4:R11)</f>
         <v>20447.076036801816</v>
@@ -4823,7 +4823,7 @@
         <v>19774.009140586251</v>
       </c>
     </row>
-    <row r="43" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:34" x14ac:dyDescent="0.3">
       <c r="S43" s="22">
         <v>64.456000000000003</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>644.55899999999997</v>
       </c>
     </row>
-    <row r="44" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:34" x14ac:dyDescent="0.3">
       <c r="S44" s="22"/>
       <c r="T44" s="22"/>
       <c r="U44" s="22"/>
@@ -4859,7 +4859,7 @@
       <c r="Y44" s="22"/>
       <c r="Z44" s="22"/>
     </row>
-    <row r="45" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:34" x14ac:dyDescent="0.3">
       <c r="AA45" s="22"/>
       <c r="AB45" s="22"/>
       <c r="AC45" s="22"/>
@@ -4869,7 +4869,7 @@
       <c r="AG45" s="22"/>
       <c r="AH45" s="22"/>
     </row>
-    <row r="46" spans="8:34" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:34" x14ac:dyDescent="0.3">
       <c r="AA46" s="22"/>
       <c r="AB46" s="22"/>
       <c r="AC46" s="22"/>

</xml_diff>